<commit_message>
Extended operation input files 'OperationScenario_BehaviorProfile.xlsx', 'OperationScenario_Component_Behavior.xlsx', 'OperationScenario.xlsx' with additional Behavioral Scenarios. Now complete (Scenario 1 - 9).
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario.xlsx
+++ b/data/input_operation/OperationScenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX/data/input_operation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevanskorna/PycharmProjects/FLEX/data/input_operation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F156E2-3A3C-EB43-983D-2C85C2D915E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DF1EB4-DDCF-2C4A-9C7E-8E4689C4BA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="-21100" windowWidth="30240" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-760" yWindow="-18800" windowWidth="30240" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -422,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="208" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -605,6 +605,252 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>